<commit_message>
Inclusão de botão para filtrar o grafico
</commit_message>
<xml_diff>
--- a/Base_de_dados.xlsx
+++ b/Base_de_dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paulo Maia\Desktop\Projeto 3 Dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E2BA72EF-B2B1-4FF3-913C-22C83D3CE3BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E287D9AC-C2CA-4C39-9C74-231155543B02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2325" yWindow="1605" windowWidth="15375" windowHeight="7785" xr2:uid="{122907A9-7D96-44C3-995C-326B71294922}"/>
+    <workbookView xWindow="23310" yWindow="1845" windowWidth="15375" windowHeight="7785" xr2:uid="{122907A9-7D96-44C3-995C-326B71294922}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -471,8 +471,9 @@
   <cols>
     <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="4" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" style="2" customWidth="1"/>
     <col min="7" max="7" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>